<commit_message>
Creating a common data provider
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -8,14 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>firstname</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Deepender Singh</t>
+  </si>
+  <si>
+    <t>Rupee</t>
   </si>
 </sst>
 </file>
@@ -390,6 +402,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -431,6 +446,37 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setting up the run mode for test suite
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="6585"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId2"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>firstname</t>
   </si>
@@ -54,6 +55,27 @@
   </si>
   <si>
     <t>Rupee</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -395,9 +417,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -454,7 +526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
skipping the testcase using runmode of the test data
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="6585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21450" windowHeight="6585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>firstname</t>
   </si>
@@ -51,9 +51,6 @@
     <t>currency</t>
   </si>
   <si>
-    <t>Deepender Singh</t>
-  </si>
-  <si>
     <t>Rupee</t>
   </si>
   <si>
@@ -75,7 +72,13 @@
     <t>Y</t>
   </si>
   <si>
+    <t>runmode</t>
+  </si>
+  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Rahul Jadhwani</t>
   </si>
 </sst>
 </file>
@@ -419,45 +422,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -467,57 +470,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>411057</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>411057</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -531,7 +543,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,10 +561,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implimenting hashmap to fetch the data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>firstname</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>runmode</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Rahul Jadhwani</t>
@@ -473,7 +470,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +498,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -561,7 +558,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
checking jenkis github build
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>firstname</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Rahul Jadhwani</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Creating pages and test for twitter login
</commit_message>
<xml_diff>
--- a/src/test/resources/excels/testdata.xlsx
+++ b/src/test/resources/excels/testdata.xlsx
@@ -12,11 +12,12 @@
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>firstname</t>
   </si>
@@ -27,58 +28,61 @@
     <t>postcode</t>
   </si>
   <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Jadhwani</t>
+  </si>
+  <si>
+    <t>alerttext</t>
+  </si>
+  <si>
+    <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>Rahul Jadhwani</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TwtLoginTest</t>
+  </si>
+  <si>
     <t>Deepender</t>
   </si>
   <si>
     <t>Singh</t>
-  </si>
-  <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Jadhwani</t>
-  </si>
-  <si>
-    <t>alerttext</t>
-  </si>
-  <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Rupee</t>
-  </si>
-  <si>
-    <t>TCID</t>
-  </si>
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>runmode</t>
-  </si>
-  <si>
-    <t>Rahul Jadhwani</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -420,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,34 +437,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +485,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +496,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -496,12 +508,12 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -513,24 +525,24 @@
         <v>411057</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>411057</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -553,18 +565,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>